<commit_message>
single host running methode changed
</commit_message>
<xml_diff>
--- a/input_file/test.xlsx
+++ b/input_file/test.xlsx
@@ -43,9 +43,6 @@
     <t>function</t>
   </si>
   <si>
-    <t>{"username":"cisco","password":"cisco","timeout":10}</t>
-  </si>
-  <si>
     <t>10.1.1.2</t>
   </si>
   <si>
@@ -74,6 +71,9 @@
   </si>
   <si>
     <t>[{"regex":{"result":"failed"},"score":0},{"regex":{"result":"success"},"score":100}]</t>
+  </si>
+  <si>
+    <t>{"username":"cisco","password":"cisco","timeout":10,"type":"cisco"}</t>
   </si>
 </sst>
 </file>
@@ -909,7 +909,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,16 +940,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -957,16 +957,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
@@ -974,16 +974,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -991,16 +991,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
@@ -1008,16 +1008,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
@@ -1025,16 +1025,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
@@ -1042,16 +1042,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
@@ -1059,16 +1059,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
@@ -1076,19 +1076,19 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>17</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>18</v>
-      </c>
-      <c r="E10" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rank inserted as string in DB not as JSON
</commit_message>
<xml_diff>
--- a/input_file/test.xlsx
+++ b/input_file/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="21">
   <si>
     <t>Hostname</t>
   </si>
@@ -28,15 +28,9 @@
     <t>rank</t>
   </si>
   <si>
-    <t>[{"regex":{"status":"down"},"score":0},{"regex":{"status":"reachable"},"score":100}]</t>
-  </si>
-  <si>
     <t>cis_sw_int</t>
   </si>
   <si>
-    <t>[{"regex":{"interface":"down"},"score":0},{"regex":{"interface":"up"},"score":100}]</t>
-  </si>
-  <si>
     <t>input</t>
   </si>
   <si>
@@ -70,10 +64,19 @@
     <t>{"cmd":"show clock,show run,show clock,show tech,show clock"}</t>
   </si>
   <si>
-    <t>[{"regex":{"result":"failed"},"score":0},{"regex":{"result":"success"},"score":100}]</t>
-  </si>
-  <si>
     <t>{"username":"cisco","password":"cisco","timeout":10,"type":"cisco"}</t>
+  </si>
+  <si>
+    <t>[{"query":{"status":{"$ne":"reachable"}},"score":0},{"query":{"status":"reachable"},"score":100}]</t>
+  </si>
+  <si>
+    <t>[{"query":{"interface":"down"},"score":0},{"query":{"interface":"up"},"score":100}]</t>
+  </si>
+  <si>
+    <t>[{"query":{"status":"down"},"score":0},{"query":{"status":"reachable"},"score":100}]</t>
+  </si>
+  <si>
+    <t>[{"query":{"result":"failed"},"score":0},{"query":{"result":"success"},"score":100}]</t>
   </si>
 </sst>
 </file>
@@ -909,7 +912,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,10 +932,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -940,155 +943,155 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
         <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>